<commit_message>
search finished, average precision calculated, missing TF_IDF & Frequency algorithm
</commit_message>
<xml_diff>
--- a/static/benchmark/benchmark.xlsx
+++ b/static/benchmark/benchmark.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giova\progetto-gestione\static\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBACED8B-A654-4AC7-B17A-F5A490884C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA98BBC6-8D38-44D0-BE35-197A9C03F8C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EB62F2A6-F713-4B85-9AF1-D20E51073B06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EB62F2A6-F713-4B85-9AF1-D20E51073B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Ricerche" sheetId="1" r:id="rId1"/>
-    <sheet name="Precision" sheetId="2" r:id="rId2"/>
+    <sheet name="Precision" sheetId="4" r:id="rId2"/>
+    <sheet name="Average Precision" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="156">
   <si>
     <t>Google</t>
   </si>
@@ -233,9 +234,6 @@
     <t>Patate al forno</t>
   </si>
   <si>
-    <t>categoria:</t>
-  </si>
-  <si>
     <t>#pizza NOT (patatine OR salame)</t>
   </si>
   <si>
@@ -366,6 +364,147 @@
   </si>
   <si>
     <t>categoria:antipasti OR contorno</t>
+  </si>
+  <si>
+    <t>Nachos caldi al formaggio</t>
+  </si>
+  <si>
+    <t>Come si preparano le olive all'ascolana</t>
+  </si>
+  <si>
+    <t>Ostriche con aceto allo scalogno</t>
+  </si>
+  <si>
+    <t>Peperoni con feta e acciughe</t>
+  </si>
+  <si>
+    <t>Crostoni al paté di carne</t>
+  </si>
+  <si>
+    <t>Dressing per pinzimonio</t>
+  </si>
+  <si>
+    <t>Antipasti nei vasetti</t>
+  </si>
+  <si>
+    <t>Tartare di verdure miste</t>
+  </si>
+  <si>
+    <t>Involtini di prosciutto cotto in gelatina al limone</t>
+  </si>
+  <si>
+    <t>Polpettine al formaggio</t>
+  </si>
+  <si>
+    <t>Spuma di tonno e acciughe</t>
+  </si>
+  <si>
+    <t>Uova ripiene fantasia</t>
+  </si>
+  <si>
+    <t>Zucchine al profumo di menta</t>
+  </si>
+  <si>
+    <t>Salatini alle nocciole</t>
+  </si>
+  <si>
+    <t>Tartellette alle cipolle</t>
+  </si>
+  <si>
+    <t>Avocado ripieno</t>
+  </si>
+  <si>
+    <t>Capesante ai pistacchi</t>
+  </si>
+  <si>
+    <t>Il paté di fegato di vitello</t>
+  </si>
+  <si>
+    <t>Chips di zucchine al forno</t>
+  </si>
+  <si>
+    <t>Garusoli aglio e olio</t>
+  </si>
+  <si>
+    <t>Pizza Margherita con bufala e pomodoro fresco</t>
+  </si>
+  <si>
+    <t>Pizza Bismarck agli asparagi</t>
+  </si>
+  <si>
+    <t>Pizza capricciosa fantasia</t>
+  </si>
+  <si>
+    <t>Pizza Margherita classica bassa all'origano</t>
+  </si>
+  <si>
+    <t>Pizza con ricotta, olive verdi e pesto di pomodori secchi</t>
+  </si>
+  <si>
+    <t>categoria: pane OR pane e pizza</t>
+  </si>
+  <si>
+    <t>Panini semidolci</t>
+  </si>
+  <si>
+    <t>Pizza alle verdure grigliate</t>
+  </si>
+  <si>
+    <t>Piadina alle zucchine</t>
+  </si>
+  <si>
+    <t>Focaccia con pomodorini</t>
+  </si>
+  <si>
+    <t>Focaccia con stracchino</t>
+  </si>
+  <si>
+    <t>Panini imbottiti</t>
+  </si>
+  <si>
+    <t>Porcellino di pizza con prosciutto,salame e wurstel</t>
+  </si>
+  <si>
+    <t>Torta o pizza al testo</t>
+  </si>
+  <si>
+    <t>Pizza con cipolle e gorgonzola</t>
+  </si>
+  <si>
+    <t>Focaccia con olive</t>
+  </si>
+  <si>
+    <t>Tortillas alla messicana</t>
+  </si>
+  <si>
+    <t>Bruschette al radicchio</t>
+  </si>
+  <si>
+    <t>Bruschettine con cicoria e salsiccia</t>
+  </si>
+  <si>
+    <t>Panini nordici al pesce affumicato</t>
+  </si>
+  <si>
+    <t>Panzerotti leggeri</t>
+  </si>
+  <si>
+    <t>Focaccine farcite</t>
+  </si>
+  <si>
+    <t>Landbrot o pane nero della Germania</t>
+  </si>
+  <si>
+    <t>Pizzette miste di pasta sfoglia</t>
+  </si>
+  <si>
+    <t>Corona di paninetti con semi di cumino</t>
+  </si>
+  <si>
+    <t>Schiacciata di speck e stracchino</t>
+  </si>
+  <si>
+    <t>categoria:pane OR pane e pizza</t>
   </si>
 </sst>
 </file>
@@ -415,17 +554,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -742,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{418C6696-A70E-4DD0-ADC0-002D58790736}">
   <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,8 +892,8 @@
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="3" width="43.5703125" customWidth="1"/>
     <col min="4" max="4" width="43.85546875" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -985,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,19 +1151,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1030,19 +1171,19 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1050,19 +1191,19 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1070,19 +1211,19 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1090,19 +1231,19 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1110,19 +1251,19 @@
         <v>6</v>
       </c>
       <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1130,19 +1271,19 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C22" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1150,19 +1291,19 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>103</v>
-      </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1170,19 +1311,19 @@
         <v>9</v>
       </c>
       <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,19 +1331,19 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,7 +1624,7 @@
       <c r="A44">
         <v>2</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C44" t="s">
@@ -1751,7 +1892,7 @@
       <c r="B59" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D59" t="s">
@@ -1889,7 +2030,7 @@
         <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1912,59 +2053,209 @@
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" t="s">
+        <v>135</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E69" t="s">
+        <v>135</v>
+      </c>
+      <c r="F69" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
+      <c r="B70" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E70" t="s">
+        <v>136</v>
+      </c>
+      <c r="F70" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>3</v>
       </c>
+      <c r="B71" t="s">
+        <v>137</v>
+      </c>
+      <c r="C71" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>4</v>
       </c>
+      <c r="B72" t="s">
+        <v>138</v>
+      </c>
+      <c r="C72" t="s">
+        <v>138</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E72" t="s">
+        <v>138</v>
+      </c>
+      <c r="F72" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5</v>
       </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" t="s">
+        <v>139</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E73" t="s">
+        <v>139</v>
+      </c>
+      <c r="F73" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>6</v>
       </c>
+      <c r="B74" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" t="s">
+        <v>140</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E74" t="s">
+        <v>140</v>
+      </c>
+      <c r="F74" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>7</v>
       </c>
+      <c r="B75" t="s">
+        <v>154</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>8</v>
       </c>
+      <c r="B76" t="s">
+        <v>142</v>
+      </c>
+      <c r="C76" t="s">
+        <v>142</v>
+      </c>
+      <c r="D76" t="s">
+        <v>151</v>
+      </c>
+      <c r="E76" t="s">
+        <v>142</v>
+      </c>
+      <c r="F76" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9</v>
       </c>
+      <c r="B77" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" t="s">
+        <v>143</v>
+      </c>
+      <c r="D77" t="s">
+        <v>152</v>
+      </c>
+      <c r="E77" t="s">
+        <v>143</v>
+      </c>
+      <c r="F77" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>10</v>
       </c>
+      <c r="B78" t="s">
+        <v>144</v>
+      </c>
+      <c r="C78" t="s">
+        <v>144</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E78" t="s">
+        <v>144</v>
+      </c>
+      <c r="F78" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>5</v>
       </c>
       <c r="B80" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1987,59 +2278,209 @@
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1</v>
+      </c>
+      <c r="B82" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2</v>
       </c>
+      <c r="B83" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E83" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>3</v>
       </c>
+      <c r="B84" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>4</v>
       </c>
+      <c r="B85" t="s">
+        <v>112</v>
+      </c>
+      <c r="C85" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E85" t="s">
+        <v>112</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>5</v>
       </c>
+      <c r="B86" t="s">
+        <v>37</v>
+      </c>
+      <c r="C86" t="s">
+        <v>37</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E86" t="s">
+        <v>37</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>6</v>
       </c>
+      <c r="B87" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" t="s">
+        <v>113</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E87" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>7</v>
       </c>
+      <c r="B88" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" t="s">
+        <v>123</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>8</v>
       </c>
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" t="s">
+        <v>115</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E89" t="s">
+        <v>115</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9</v>
       </c>
+      <c r="B90" t="s">
+        <v>116</v>
+      </c>
+      <c r="C90" t="s">
+        <v>116</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E90" t="s">
+        <v>116</v>
+      </c>
+      <c r="F90" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>10</v>
       </c>
+      <c r="B91" t="s">
+        <v>117</v>
+      </c>
+      <c r="C91" t="s">
+        <v>117</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E91" t="s">
+        <v>117</v>
+      </c>
+      <c r="F91" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2064,19 +2505,19 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
+        <v>82</v>
+      </c>
+      <c r="C95" t="s">
+        <v>82</v>
+      </c>
+      <c r="D95" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C95" t="s">
-        <v>83</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="E95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2084,19 +2525,19 @@
         <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D96" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E96" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E96" s="1" t="s">
-        <v>84</v>
-      </c>
       <c r="F96" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2104,19 +2545,19 @@
         <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2124,19 +2565,19 @@
         <v>4</v>
       </c>
       <c r="B98" t="s">
-        <v>94</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>86</v>
+        <v>93</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2144,19 +2585,19 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D99" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2164,19 +2605,19 @@
         <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D100" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,19 +2625,19 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F101" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2204,19 +2645,19 @@
         <v>8</v>
       </c>
       <c r="B102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F102" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2224,19 +2665,19 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F103" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2244,19 +2685,19 @@
         <v>10</v>
       </c>
       <c r="B104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F104" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2264,7 +2705,7 @@
         <v>5</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -2287,59 +2728,209 @@
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1</v>
+      </c>
+      <c r="B108" t="s">
+        <v>67</v>
+      </c>
+      <c r="C108" t="s">
+        <v>67</v>
+      </c>
+      <c r="D108" t="s">
+        <v>67</v>
+      </c>
+      <c r="E108" t="s">
+        <v>67</v>
+      </c>
+      <c r="F108" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2</v>
       </c>
+      <c r="B109" t="s">
+        <v>75</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>3</v>
       </c>
+      <c r="B110" t="s">
+        <v>130</v>
+      </c>
+      <c r="C110" t="s">
+        <v>130</v>
+      </c>
+      <c r="D110" t="s">
+        <v>130</v>
+      </c>
+      <c r="E110" t="s">
+        <v>130</v>
+      </c>
+      <c r="F110" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>4</v>
       </c>
+      <c r="B111" t="s">
+        <v>69</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" t="s">
+        <v>131</v>
+      </c>
+      <c r="E111" t="s">
+        <v>69</v>
+      </c>
+      <c r="F111" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>5</v>
       </c>
+      <c r="B112" t="s">
+        <v>131</v>
+      </c>
+      <c r="C112" t="s">
+        <v>131</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E112" t="s">
+        <v>131</v>
+      </c>
+      <c r="F112" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>6</v>
       </c>
+      <c r="B113" t="s">
+        <v>132</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D113" t="s">
+        <v>132</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>7</v>
       </c>
+      <c r="B114" t="s">
+        <v>70</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D114" t="s">
+        <v>70</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>8</v>
       </c>
+      <c r="B115" t="s">
+        <v>72</v>
+      </c>
+      <c r="C115" t="s">
+        <v>72</v>
+      </c>
+      <c r="D115" t="s">
+        <v>72</v>
+      </c>
+      <c r="E115" t="s">
+        <v>72</v>
+      </c>
+      <c r="F115" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>9</v>
       </c>
+      <c r="B116" t="s">
+        <v>73</v>
+      </c>
+      <c r="C116" t="s">
+        <v>73</v>
+      </c>
+      <c r="D116" t="s">
+        <v>73</v>
+      </c>
+      <c r="E116" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>10</v>
       </c>
+      <c r="B117" t="s">
+        <v>74</v>
+      </c>
+      <c r="C117" t="s">
+        <v>74</v>
+      </c>
+      <c r="D117" t="s">
+        <v>74</v>
+      </c>
+      <c r="E117" t="s">
+        <v>133</v>
+      </c>
+      <c r="F117" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>5</v>
       </c>
       <c r="B119" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -2364,19 +2955,19 @@
         <v>1</v>
       </c>
       <c r="B121" t="s">
+        <v>67</v>
+      </c>
+      <c r="C121" t="s">
+        <v>67</v>
+      </c>
+      <c r="D121" t="s">
+        <v>67</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C121" t="s">
-        <v>68</v>
-      </c>
-      <c r="D121" t="s">
-        <v>68</v>
-      </c>
-      <c r="E121" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="F121" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -2384,19 +2975,19 @@
         <v>2</v>
       </c>
       <c r="B122" t="s">
+        <v>68</v>
+      </c>
+      <c r="C122" t="s">
+        <v>68</v>
+      </c>
+      <c r="D122" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C122" t="s">
+      <c r="E122" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F122" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E122" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F122" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -2404,19 +2995,19 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
+        <v>69</v>
+      </c>
+      <c r="C123" t="s">
+        <v>69</v>
+      </c>
+      <c r="D123" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C123" t="s">
-        <v>70</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E123" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -2424,19 +3015,19 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
+        <v>70</v>
+      </c>
+      <c r="C124" t="s">
+        <v>70</v>
+      </c>
+      <c r="D124" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C124" t="s">
-        <v>71</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="E124" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F124" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -2444,19 +3035,19 @@
         <v>5</v>
       </c>
       <c r="B125" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C125" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D125" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D125" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E125" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -2464,19 +3055,19 @@
         <v>6</v>
       </c>
       <c r="B126" t="s">
+        <v>72</v>
+      </c>
+      <c r="C126" t="s">
+        <v>72</v>
+      </c>
+      <c r="D126" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C126" t="s">
-        <v>73</v>
-      </c>
-      <c r="D126" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -2484,19 +3075,19 @@
         <v>7</v>
       </c>
       <c r="B127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F127" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -2504,19 +3095,19 @@
         <v>8</v>
       </c>
       <c r="B128" t="s">
+        <v>74</v>
+      </c>
+      <c r="C128" t="s">
+        <v>74</v>
+      </c>
+      <c r="D128" t="s">
+        <v>74</v>
+      </c>
+      <c r="E128" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C128" t="s">
+      <c r="F128" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="D128" t="s">
-        <v>75</v>
-      </c>
-      <c r="E128" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F128" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -2524,19 +3115,19 @@
         <v>9</v>
       </c>
       <c r="B129" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C129" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D129" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -2544,19 +3135,19 @@
         <v>10</v>
       </c>
       <c r="B130" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C130" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D130" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D130" s="1" t="s">
+      <c r="E130" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E130" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F130" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2566,78 +3157,70 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679849B1-0895-4B0F-9F27-9AD6972CD93B}">
-  <dimension ref="A1:J64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44764E0C-A0DF-4545-A40E-1065B4949820}">
+  <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4" t="s">
+      <c r="A1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="4"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="B3" s="6">
         <v>0.1</v>
       </c>
       <c r="C3">
@@ -2670,7 +3253,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>0.2</v>
       </c>
       <c r="C4">
@@ -2703,7 +3286,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="B5" s="6">
         <v>0.3</v>
       </c>
       <c r="C5">
@@ -2736,7 +3319,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="B6" s="6">
         <v>0.4</v>
       </c>
       <c r="C6">
@@ -2769,7 +3352,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="B7" s="6">
         <v>0.5</v>
       </c>
       <c r="C7">
@@ -2802,7 +3385,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="B8" s="6">
         <v>0.6</v>
       </c>
       <c r="C8">
@@ -2835,7 +3418,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="B9" s="6">
         <v>0.7</v>
       </c>
       <c r="C9">
@@ -2868,7 +3451,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="B10" s="6">
         <v>0.8</v>
       </c>
       <c r="C10">
@@ -2901,7 +3484,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="B11" s="6">
         <v>0.9</v>
       </c>
       <c r="C11">
@@ -2934,7 +3517,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="B12" s="6">
         <v>1</v>
       </c>
       <c r="C12">
@@ -2967,60 +3550,60 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
+      <c r="A14" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4" t="s">
+      <c r="H14" s="8"/>
+      <c r="I14" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="4"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="B16" s="6">
         <v>0.1</v>
       </c>
       <c r="C16">
@@ -3053,7 +3636,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="B17" s="6">
         <v>0.2</v>
       </c>
       <c r="C17">
@@ -3086,7 +3669,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="6">
         <v>0.3</v>
       </c>
       <c r="C18">
@@ -3119,7 +3702,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="6">
         <v>0.4</v>
       </c>
       <c r="C19">
@@ -3152,7 +3735,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="6">
         <v>0.5</v>
       </c>
       <c r="C20">
@@ -3185,7 +3768,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="B21" s="6">
         <v>0.6</v>
       </c>
       <c r="C21">
@@ -3218,7 +3801,7 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="B22" s="6">
         <v>0.7</v>
       </c>
       <c r="C22">
@@ -3251,7 +3834,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="B23" s="6">
         <v>0.8</v>
       </c>
       <c r="C23">
@@ -3284,7 +3867,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="2">
+      <c r="B24" s="6">
         <v>0.9</v>
       </c>
       <c r="C24">
@@ -3317,7 +3900,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="2">
+      <c r="B25" s="6">
         <v>1</v>
       </c>
       <c r="C25">
@@ -3350,60 +3933,60 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="4" t="s">
+      <c r="A27" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4" t="s">
+      <c r="F27" s="8"/>
+      <c r="G27" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="4"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="H28" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I28" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
+      <c r="B29" s="6">
         <v>0.1</v>
       </c>
       <c r="C29">
@@ -3436,7 +4019,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="2">
+      <c r="B30" s="6">
         <v>0.2</v>
       </c>
       <c r="C30">
@@ -3469,7 +4052,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="2">
+      <c r="B31" s="6">
         <v>0.3</v>
       </c>
       <c r="C31">
@@ -3502,7 +4085,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
+      <c r="B32" s="6">
         <v>0.4</v>
       </c>
       <c r="C32">
@@ -3535,7 +4118,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="2">
+      <c r="B33" s="6">
         <v>0.5</v>
       </c>
       <c r="C33">
@@ -3568,7 +4151,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="2">
+      <c r="B34" s="6">
         <v>0.6</v>
       </c>
       <c r="C34">
@@ -3601,7 +4184,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
+      <c r="B35" s="6">
         <v>0.7</v>
       </c>
       <c r="C35">
@@ -3634,7 +4217,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+      <c r="B36" s="6">
         <v>0.8</v>
       </c>
       <c r="C36">
@@ -3667,7 +4250,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="2">
+      <c r="B37" s="6">
         <v>0.9</v>
       </c>
       <c r="C37">
@@ -3700,7 +4283,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
+      <c r="B38" s="6">
         <v>1</v>
       </c>
       <c r="C38">
@@ -3733,60 +4316,60 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="4" t="s">
+      <c r="A40" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H40" s="4"/>
-      <c r="I40" s="4" t="s">
+      <c r="H40" s="8"/>
+      <c r="I40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J40" s="4"/>
+      <c r="J40" s="8"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="I41" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="J41" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="2">
+      <c r="B42" s="6">
         <v>0.1</v>
       </c>
       <c r="C42">
@@ -3819,7 +4402,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="2">
+      <c r="B43" s="6">
         <v>0.2</v>
       </c>
       <c r="C43">
@@ -3852,7 +4435,7 @@
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B44" s="2">
+      <c r="B44" s="6">
         <v>0.3</v>
       </c>
       <c r="C44">
@@ -3885,7 +4468,7 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B45" s="2">
+      <c r="B45" s="6">
         <v>0.4</v>
       </c>
       <c r="C45">
@@ -3918,7 +4501,7 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B46" s="2">
+      <c r="B46" s="6">
         <v>0.5</v>
       </c>
       <c r="C46">
@@ -3951,7 +4534,7 @@
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B47" s="2">
+      <c r="B47" s="6">
         <v>0.6</v>
       </c>
       <c r="C47">
@@ -3984,7 +4567,7 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B48" s="2">
+      <c r="B48" s="6">
         <v>0.7</v>
       </c>
       <c r="C48">
@@ -4017,7 +4600,7 @@
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B49" s="2">
+      <c r="B49" s="6">
         <v>0.8</v>
       </c>
       <c r="C49">
@@ -4050,7 +4633,7 @@
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B50" s="2">
+      <c r="B50" s="6">
         <v>0.9</v>
       </c>
       <c r="C50">
@@ -4083,7 +4666,7 @@
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B51" s="2">
+      <c r="B51" s="6">
         <v>1</v>
       </c>
       <c r="C51">
@@ -4116,60 +4699,60 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="4" t="s">
+      <c r="A53" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4" t="s">
+      <c r="F53" s="8"/>
+      <c r="G53" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4" t="s">
+      <c r="H53" s="8"/>
+      <c r="I53" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J53" s="4"/>
+      <c r="J53" s="8"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="E54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="F54" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="G54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="H54" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J54" s="2" t="s">
+      <c r="J54" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="2">
+      <c r="B55" s="6">
         <v>0.1</v>
       </c>
       <c r="C55">
@@ -4202,7 +4785,7 @@
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B56" s="2">
+      <c r="B56" s="6">
         <v>0.2</v>
       </c>
       <c r="C56">
@@ -4235,7 +4818,7 @@
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B57" s="2">
+      <c r="B57" s="6">
         <v>0.3</v>
       </c>
       <c r="C57">
@@ -4249,7 +4832,7 @@
         <v>6</v>
       </c>
       <c r="F57">
-        <f t="shared" ref="F56:F64" si="19">IF(E57=0,0,(B44*10)/E57)</f>
+        <f t="shared" ref="F57:F64" si="19">IF(E57=0,0,(B44*10)/E57)</f>
         <v>0.5</v>
       </c>
       <c r="G57">
@@ -4268,7 +4851,7 @@
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B58" s="2">
+      <c r="B58" s="6">
         <v>0.4</v>
       </c>
       <c r="C58">
@@ -4301,7 +4884,7 @@
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B59" s="2">
+      <c r="B59" s="6">
         <v>0.5</v>
       </c>
       <c r="C59">
@@ -4334,7 +4917,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B60" s="2">
+      <c r="B60" s="6">
         <v>0.6</v>
       </c>
       <c r="C60">
@@ -4367,7 +4950,7 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B61" s="2">
+      <c r="B61" s="6">
         <v>0.7</v>
       </c>
       <c r="C61">
@@ -4400,7 +4983,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B62" s="2">
+      <c r="B62" s="6">
         <v>0.8</v>
       </c>
       <c r="C62">
@@ -4430,7 +5013,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B63" s="2">
+      <c r="B63" s="6">
         <v>0.9</v>
       </c>
       <c r="C63">
@@ -4460,7 +5043,7 @@
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B64" s="2">
+      <c r="B64" s="6">
         <v>1</v>
       </c>
       <c r="C64">
@@ -4489,12 +5072,1947 @@
         <v>0</v>
       </c>
     </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="8"/>
+      <c r="G66" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J66" s="8"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>155</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <f>IF(C68=0,0,(B55*10)/C68)</f>
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>8</v>
+      </c>
+      <c r="F68">
+        <f>IF(E68=0,0,(B55*10)/E68)</f>
+        <v>0.125</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <f>IF(G68=0,0,(B55*10)/G68)</f>
+        <v>1</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <f>IF(I68=0,0,(B55*10)/I68)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <f t="shared" ref="D69:D77" si="20">IF(C69=0,0,(B56*10)/C69)</f>
+        <v>1</v>
+      </c>
+      <c r="E69">
+        <v>9</v>
+      </c>
+      <c r="F69">
+        <f>IF(E69=0,0,(B56*10)/E69)</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="G69">
+        <v>2</v>
+      </c>
+      <c r="H69">
+        <f t="shared" ref="H69:H77" si="21">IF(G69=0,0,(B56*10)/G69)</f>
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>2</v>
+      </c>
+      <c r="J69">
+        <f t="shared" ref="J69:J77" si="22">IF(I69=0,0,(B56*10)/I69)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C70">
+        <v>3</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <f t="shared" ref="F70:F77" si="23">IF(E70=0,0,(B57*10)/E70)</f>
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>3</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="I70">
+        <v>3</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>4</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C72">
+        <v>5</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="I72">
+        <v>5</v>
+      </c>
+      <c r="J72">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C73">
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>6</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>6</v>
+      </c>
+      <c r="J73">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C74">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="20"/>
+        <v>0.875</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>8</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="21"/>
+        <v>0.875</v>
+      </c>
+      <c r="I74">
+        <v>8</v>
+      </c>
+      <c r="J74">
+        <f t="shared" si="22"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C75">
+        <v>9</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="20"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>9</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="21"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="I75">
+        <v>9</v>
+      </c>
+      <c r="J75">
+        <f t="shared" si="22"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="20"/>
+        <v>0.9</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>10</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="21"/>
+        <v>0.9</v>
+      </c>
+      <c r="I76">
+        <v>10</v>
+      </c>
+      <c r="J76">
+        <f t="shared" si="22"/>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="6">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>0</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F79" s="8"/>
+      <c r="G79" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J79" s="8"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <f>IF(C81=0,0,(B68*10)/C81)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E81">
+        <v>7</v>
+      </c>
+      <c r="F81">
+        <f>IF(E81=0,0,(B68*10)/E81)</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="G81">
+        <v>2</v>
+      </c>
+      <c r="H81">
+        <f>IF(G81=0,0,(B68*10)/G81)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I81">
+        <v>9</v>
+      </c>
+      <c r="J81">
+        <f>IF(I81=0,0,(B68*10)/I81)</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B82" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C82">
+        <v>4</v>
+      </c>
+      <c r="D82">
+        <f t="shared" ref="D82:D90" si="24">IF(C82=0,0,(B69*10)/C82)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <f>IF(E82=0,0,(B69*10)/E82)</f>
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>4</v>
+      </c>
+      <c r="H82">
+        <f t="shared" ref="H82:H90" si="25">IF(G82=0,0,(B69*10)/G82)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I82">
+        <v>10</v>
+      </c>
+      <c r="J82">
+        <f t="shared" ref="J82:J90" si="26">IF(I82=0,0,(B69*10)/I82)</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C83">
+        <v>5</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="24"/>
+        <v>0.6</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <f t="shared" ref="F83:F90" si="27">IF(E83=0,0,(B70*10)/E83)</f>
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>5</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="25"/>
+        <v>0.6</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C84">
+        <v>6</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="24"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>6</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C85">
+        <v>8</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="24"/>
+        <v>0.625</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>8</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="25"/>
+        <v>0.625</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C86">
+        <v>9</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="24"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>9</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="25"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B87" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="24"/>
+        <v>0.7</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>10</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="25"/>
+        <v>0.7</v>
+      </c>
+      <c r="I87">
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B88" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B89" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>0</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="6">
+        <v>1</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J92" s="8"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I93" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J93" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B94" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <f>IF(C94=0,0,(B81*10)/C94)</f>
+        <v>1</v>
+      </c>
+      <c r="E94">
+        <v>3</v>
+      </c>
+      <c r="F94">
+        <f>IF(E94=0,0,(B81*10)/E94)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G94">
+        <v>1</v>
+      </c>
+      <c r="H94">
+        <f>IF(G94=0,0,(B81*10)/G94)</f>
+        <v>1</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <f>IF(I94=0,0,(B81*10)/I94)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B95" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C95">
+        <v>3</v>
+      </c>
+      <c r="D95">
+        <f t="shared" ref="D95:D103" si="28">IF(C95=0,0,(B82*10)/C95)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E95">
+        <v>5</v>
+      </c>
+      <c r="F95">
+        <f>IF(E95=0,0,(B82*10)/E95)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G95">
+        <v>3</v>
+      </c>
+      <c r="H95">
+        <f t="shared" ref="H95:H103" si="29">IF(G95=0,0,(B82*10)/G95)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I95">
+        <v>3</v>
+      </c>
+      <c r="J95">
+        <f t="shared" ref="J95:J103" si="30">IF(I95=0,0,(B82*10)/I95)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B96" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="28"/>
+        <v>0.6</v>
+      </c>
+      <c r="E96">
+        <v>6</v>
+      </c>
+      <c r="F96">
+        <f t="shared" ref="F96:F103" si="31">IF(E96=0,0,(B83*10)/E96)</f>
+        <v>0.5</v>
+      </c>
+      <c r="G96">
+        <v>7</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="29"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="I96">
+        <v>7</v>
+      </c>
+      <c r="J96">
+        <f t="shared" si="30"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B97" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C97">
+        <v>6</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="28"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E97">
+        <v>7</v>
+      </c>
+      <c r="F97">
+        <f t="shared" si="31"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G97">
+        <v>8</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="29"/>
+        <v>0.5</v>
+      </c>
+      <c r="I97">
+        <v>8</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="30"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B98" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C98">
+        <v>7</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="28"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="E98">
+        <v>8</v>
+      </c>
+      <c r="F98">
+        <f t="shared" si="31"/>
+        <v>0.625</v>
+      </c>
+      <c r="G98">
+        <v>9</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="29"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="I98">
+        <v>9</v>
+      </c>
+      <c r="J98">
+        <f t="shared" si="30"/>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B99" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C99">
+        <v>8</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="28"/>
+        <v>0.75</v>
+      </c>
+      <c r="E99">
+        <v>9</v>
+      </c>
+      <c r="F99">
+        <f t="shared" si="31"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G99">
+        <v>10</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="29"/>
+        <v>0.6</v>
+      </c>
+      <c r="I99">
+        <v>10</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="30"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B100" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C100">
+        <v>9</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="28"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E100">
+        <v>10</v>
+      </c>
+      <c r="F100">
+        <f t="shared" si="31"/>
+        <v>0.7</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I100">
+        <v>0</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B101" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="28"/>
+        <v>0.8</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B102" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I102">
+        <v>0</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B103" s="6">
+        <v>1</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" s="7"/>
+      <c r="E105" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F105" s="8"/>
+      <c r="G105" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J105" s="8"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>65</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J106" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B107" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C107">
+        <v>1</v>
+      </c>
+      <c r="D107">
+        <f>IF(C107=0,0,(B94*10)/C107)</f>
+        <v>1</v>
+      </c>
+      <c r="E107">
+        <v>1</v>
+      </c>
+      <c r="F107">
+        <f>IF(E107=0,0,(B94*10)/E107)</f>
+        <v>1</v>
+      </c>
+      <c r="G107">
+        <v>1</v>
+      </c>
+      <c r="H107">
+        <f>IF(G107=0,0,(B94*10)/G107)</f>
+        <v>1</v>
+      </c>
+      <c r="I107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <f>IF(I107=0,0,(B94*10)/I107)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B108" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C108">
+        <v>3</v>
+      </c>
+      <c r="D108">
+        <f t="shared" ref="D108:D116" si="32">IF(C108=0,0,(B95*10)/C108)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E108">
+        <v>3</v>
+      </c>
+      <c r="F108">
+        <f>IF(E108=0,0,(B95*10)/E108)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G108">
+        <v>3</v>
+      </c>
+      <c r="H108">
+        <f t="shared" ref="H108:H116" si="33">IF(G108=0,0,(B95*10)/G108)</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="I108">
+        <v>3</v>
+      </c>
+      <c r="J108">
+        <f t="shared" ref="J108:J116" si="34">IF(I108=0,0,(B95*10)/I108)</f>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B109" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C109">
+        <v>4</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="32"/>
+        <v>0.75</v>
+      </c>
+      <c r="E109">
+        <v>4</v>
+      </c>
+      <c r="F109">
+        <f t="shared" ref="F109:F116" si="35">IF(E109=0,0,(B96*10)/E109)</f>
+        <v>0.75</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="33"/>
+        <v>0.75</v>
+      </c>
+      <c r="I109">
+        <v>4</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="34"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B110" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C110">
+        <v>5</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="32"/>
+        <v>0.8</v>
+      </c>
+      <c r="E110">
+        <v>6</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="35"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G110">
+        <v>5</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="33"/>
+        <v>0.8</v>
+      </c>
+      <c r="I110">
+        <v>5</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="34"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B111" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C111">
+        <v>8</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="32"/>
+        <v>0.625</v>
+      </c>
+      <c r="E111">
+        <v>7</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="35"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G111">
+        <v>8</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="33"/>
+        <v>0.625</v>
+      </c>
+      <c r="I111">
+        <v>8</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="34"/>
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B112" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C112">
+        <v>9</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="32"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E112">
+        <v>8</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="35"/>
+        <v>0.75</v>
+      </c>
+      <c r="G112">
+        <v>10</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="33"/>
+        <v>0.6</v>
+      </c>
+      <c r="I112">
+        <v>10</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="34"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B113" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C113">
+        <v>10</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="32"/>
+        <v>0.7</v>
+      </c>
+      <c r="E113">
+        <v>9</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="35"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="I113">
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B114" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>10</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="35"/>
+        <v>0.8</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="I114">
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B115" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B116" s="6">
+        <v>1</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D118" s="7"/>
+      <c r="E118" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" s="8"/>
+      <c r="G118" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J118" s="8"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>66</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J119" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B120" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <f>IF(C120=0,0,(B107*10)/C120)</f>
+        <v>1</v>
+      </c>
+      <c r="E120">
+        <v>1</v>
+      </c>
+      <c r="F120">
+        <f>IF(E120=0,0,(B107*10)/E120)</f>
+        <v>1</v>
+      </c>
+      <c r="G120">
+        <v>3</v>
+      </c>
+      <c r="H120">
+        <f>IF(G120=0,0,(B107*10)/G120)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I120">
+        <v>4</v>
+      </c>
+      <c r="J120">
+        <f>IF(I120=0,0,(B107*10)/I120)</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B121" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C121">
+        <v>2</v>
+      </c>
+      <c r="D121">
+        <f t="shared" ref="D121:D129" si="36">IF(C121=0,0,(B108*10)/C121)</f>
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>8</v>
+      </c>
+      <c r="F121">
+        <f>IF(E121=0,0,(B108*10)/E121)</f>
+        <v>0.25</v>
+      </c>
+      <c r="G121">
+        <v>4</v>
+      </c>
+      <c r="H121">
+        <f t="shared" ref="H121:H129" si="37">IF(G121=0,0,(B108*10)/G121)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I121">
+        <v>6</v>
+      </c>
+      <c r="J121">
+        <f t="shared" ref="J121:J129" si="38">IF(I121=0,0,(B108*10)/I121)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B122" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
+      </c>
+      <c r="D122">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="E122">
+        <v>9</v>
+      </c>
+      <c r="F122">
+        <f t="shared" ref="F122:F129" si="39">IF(E122=0,0,(B109*10)/E122)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G122">
+        <v>6</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="37"/>
+        <v>0.5</v>
+      </c>
+      <c r="I122">
+        <v>7</v>
+      </c>
+      <c r="J122">
+        <f t="shared" si="38"/>
+        <v>0.42857142857142855</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B123" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C123">
+        <v>4</v>
+      </c>
+      <c r="D123">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G123">
+        <v>7</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="37"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="I123">
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B124" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C124">
+        <v>6</v>
+      </c>
+      <c r="D124">
+        <f t="shared" si="36"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B125" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C125">
+        <v>7</v>
+      </c>
+      <c r="D125">
+        <f t="shared" si="36"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G125">
+        <v>0</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B126" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C126">
+        <v>8</v>
+      </c>
+      <c r="D126">
+        <f t="shared" si="36"/>
+        <v>0.875</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G126">
+        <v>0</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I126">
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B127" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C127">
+        <v>9</v>
+      </c>
+      <c r="D127">
+        <f t="shared" si="36"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G127">
+        <v>0</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B128" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B129" s="6">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="G129">
+        <v>0</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>0</v>
+      </c>
+      <c r="J129">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="40">
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="G105:H105"/>
+    <mergeCell ref="I105:J105"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="G118:H118"/>
+    <mergeCell ref="I118:J118"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="G79:H79"/>
+    <mergeCell ref="I79:J79"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="E92:F92"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="I92:J92"/>
     <mergeCell ref="C53:D53"/>
     <mergeCell ref="E53:F53"/>
     <mergeCell ref="G53:H53"/>
     <mergeCell ref="I53:J53"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="I66:J66"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="G27:H27"/>
@@ -4514,4 +7032,338 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D36D598-F891-450D-A2A6-1304BD0F4638}">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="8"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="9">
+        <f>(Precision!D3+Precision!D16+Precision!D29+Precision!D42+Precision!D55+Precision!D68+Precision!D81+Precision!D94+Precision!D107+Precision!D120)/10</f>
+        <v>0.8</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9">
+        <f>(Precision!F3+Precision!F16+Precision!F29+Precision!F42+Precision!F55+Precision!F68+Precision!F81+Precision!F94+Precision!F107+Precision!F120)/10</f>
+        <v>0.61011904761904767</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9">
+        <f>(Precision!H3+Precision!H16+Precision!H29+Precision!H42+Precision!H55+Precision!H68+Precision!H81+Precision!H94+Precision!H107+Precision!H120)/10</f>
+        <v>0.73333333333333328</v>
+      </c>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9">
+        <f>(Precision!J3+Precision!J16+Precision!J29+Precision!J42+Precision!J55+Precision!J68+Precision!J81+Precision!J94+Precision!J107+Precision!J120)/10</f>
+        <v>0.68611111111111112</v>
+      </c>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="9">
+        <f>(Precision!D4+Precision!D17+Precision!D30+Precision!D43+Precision!D56+Precision!D69+Precision!D82+Precision!D95+Precision!D108+Precision!D121)/10</f>
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9">
+        <f>(Precision!F4+Precision!F17+Precision!F30+Precision!F43+Precision!F56+Precision!F69+Precision!F82+Precision!F95+Precision!F108+Precision!F121)/10</f>
+        <v>0.42055555555555557</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
+        <f>(Precision!H4+Precision!H17+Precision!H30+Precision!H43+Precision!H56+Precision!H69+Precision!H82+Precision!H95+Precision!H108+Precision!H121)/10</f>
+        <v>0.68333333333333335</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9">
+        <f>(Precision!J4+Precision!J17+Precision!J30+Precision!J43+Precision!J56+Precision!J69+Precision!J82+Precision!J95+Precision!J108+Precision!J121)/10</f>
+        <v>0.55333333333333334</v>
+      </c>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="9">
+        <f>(Precision!D5+Precision!D18+Precision!D31+Precision!D44+Precision!D57+Precision!D70+Precision!D83+Precision!D96+Precision!D109+Precision!D122)/10</f>
+        <v>0.77999999999999992</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9">
+        <f>(Precision!F5+Precision!F18+Precision!F31+Precision!F44+Precision!F57+Precision!F70+Precision!F83+Precision!F96+Precision!F109+Precision!F122)/10</f>
+        <v>0.39333333333333337</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <f>(Precision!H5+Precision!H18+Precision!H31+Precision!H44+Precision!H57+Precision!H70+Precision!H83+Precision!H96+Precision!H109+Precision!H122)/10</f>
+        <v>0.69785714285714284</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9">
+        <f>(Precision!J5+Precision!J18+Precision!J31+Precision!J44+Precision!J57+Precision!J70+Precision!J83+Precision!J96+Precision!J109+Precision!J122)/10</f>
+        <v>0.54571428571428571</v>
+      </c>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C5" s="9">
+        <f>(Precision!D6+Precision!D19+Precision!D32+Precision!D45+Precision!D58+Precision!D71+Precision!D84+Precision!D97+Precision!D110+Precision!D123)/10</f>
+        <v>0.79714285714285715</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9">
+        <f>(Precision!F6+Precision!F19+Precision!F32+Precision!F45+Precision!F58+Precision!F71+Precision!F84+Precision!F97+Precision!F110+Precision!F123)/10</f>
+        <v>0.29761904761904756</v>
+      </c>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9">
+        <f>(Precision!H6+Precision!H19+Precision!H32+Precision!H45+Precision!H58+Precision!H71+Precision!H84+Precision!H97+Precision!H110+Precision!H123)/10</f>
+        <v>0.71476190476190471</v>
+      </c>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9">
+        <f>(Precision!J6+Precision!J19+Precision!J32+Precision!J45+Precision!J58+Precision!J71+Precision!J84+Precision!J97+Precision!J110+Precision!J123)/10</f>
+        <v>0.51095238095238094</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="9">
+        <f>(Precision!D7+Precision!D20+Precision!D33+Precision!D46+Precision!D59+Precision!D72+Precision!D85+Precision!D98+Precision!D111+Precision!D124)/10</f>
+        <v>0.74285714285714288</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9">
+        <f>(Precision!F7+Precision!F20+Precision!F33+Precision!F46+Precision!F59+Precision!F72+Precision!F85+Precision!F98+Precision!F111+Precision!F124)/10</f>
+        <v>0.32341269841269843</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9">
+        <f>(Precision!H7+Precision!H20+Precision!H33+Precision!H46+Precision!H59+Precision!H72+Precision!H85+Precision!H98+Precision!H111+Precision!H124)/10</f>
+        <v>0.6436507936507937</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9">
+        <f>(Precision!J7+Precision!J20+Precision!J33+Precision!J46+Precision!J59+Precision!J72+Precision!J85+Precision!J98+Precision!J111+Precision!J124)/10</f>
+        <v>0.49781746031746038</v>
+      </c>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="9">
+        <f>(Precision!D8+Precision!D21+Precision!D34+Precision!D47+Precision!D60+Precision!D73+Precision!D86+Precision!D99+Precision!D112+Precision!D125)/10</f>
+        <v>0.77380952380952384</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9">
+        <f>(Precision!F8+Precision!F21+Precision!F34+Precision!F47+Precision!F60+Precision!F73+Precision!F86+Precision!F99+Precision!F112+Precision!F125)/10</f>
+        <v>0.28333333333333333</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <f>(Precision!H8+Precision!H21+Precision!H34+Precision!H47+Precision!H60+Precision!H73+Precision!H86+Precision!H99+Precision!H112+Precision!H125)/10</f>
+        <v>0.66642857142857137</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9">
+        <f>(Precision!J8+Precision!J21+Precision!J34+Precision!J47+Precision!J60+Precision!J73+Precision!J86+Precision!J99+Precision!J112+Precision!J125)/10</f>
+        <v>0.51404761904761898</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="C8" s="9">
+        <f>(Precision!D9+Precision!D22+Precision!D35+Precision!D48+Precision!D61+Precision!D74+Precision!D87+Precision!D100+Precision!D113+Precision!D126)/10</f>
+        <v>0.68833333333333335</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
+        <f>(Precision!F9+Precision!F22+Precision!F35+Precision!F48+Precision!F61+Precision!F74+Precision!F87+Precision!F100+Precision!F113+Precision!F126)/10</f>
+        <v>0.29555555555555557</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9">
+        <f>(Precision!H9+Precision!H22+Precision!H35+Precision!H48+Precision!H61+Precision!H74+Precision!H87+Precision!H100+Precision!H113+Precision!H126)/10</f>
+        <v>0.4530555555555556</v>
+      </c>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9">
+        <f>(Precision!J9+Precision!J22+Precision!J35+Precision!J48+Precision!J61+Precision!J74+Precision!J87+Precision!J100+Precision!J113+Precision!J126)/10</f>
+        <v>0.31305555555555553</v>
+      </c>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="C9" s="9">
+        <f>(Precision!D10+Precision!D23+Precision!D36+Precision!D49+Precision!D62+Precision!D75+Precision!D88+Precision!D101+Precision!D114+Precision!D127)/10</f>
+        <v>0.33777777777777779</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9">
+        <f>(Precision!F10+Precision!F23+Precision!F36+Precision!F49+Precision!F62+Precision!F75+Precision!F88+Precision!F101+Precision!F114+Precision!F127)/10</f>
+        <v>0.16</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <f>(Precision!H10+Precision!H23+Precision!H36+Precision!H49+Precision!H62+Precision!H75+Precision!H88+Precision!H101+Precision!H114+Precision!H127)/10</f>
+        <v>0.16888888888888889</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9">
+        <f>(Precision!J10+Precision!J23+Precision!J36+Precision!J49+Precision!J62+Precision!J75+Precision!J88+Precision!J101+Precision!J114+Precision!J127)/10</f>
+        <v>0.16888888888888889</v>
+      </c>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="C10" s="9">
+        <f>(Precision!D11+Precision!D24+Precision!D37+Precision!D50+Precision!D63+Precision!D76+Precision!D89+Precision!D102+Precision!D115+Precision!D128)/10</f>
+        <v>0.09</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9">
+        <f>(Precision!F11+Precision!F24+Precision!F37+Precision!F50+Precision!F63+Precision!F76+Precision!F89+Precision!F102+Precision!F115+Precision!F128)/10</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <f>(Precision!H11+Precision!H24+Precision!H37+Precision!H50+Precision!H63+Precision!H76+Precision!H89+Precision!H102+Precision!H115+Precision!H128)/10</f>
+        <v>0.09</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9">
+        <f>(Precision!J11+Precision!J24+Precision!J37+Precision!J50+Precision!J63+Precision!J76+Precision!J89+Precision!J102+Precision!J115+Precision!J128)/10</f>
+        <v>0.09</v>
+      </c>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <f>(Precision!D12+Precision!D25+Precision!D38+Precision!D51+Precision!D64+Precision!D77+Precision!D90+Precision!D103+Precision!D116+Precision!D129)/10</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
+        <f>(Precision!F12+Precision!F25+Precision!F38+Precision!F51+Precision!F64+Precision!F77+Precision!F90+Precision!F103+Precision!F116+Precision!F129)/10</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
+        <f>(Precision!H12+Precision!H25+Precision!H38+Precision!H51+Precision!H64+Precision!H77+Precision!H90+Precision!H103+Precision!H116+Precision!H129)/10</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9">
+        <f>(Precision!J12+Precision!J25+Precision!J38+Precision!J51+Precision!J64+Precision!J77+Precision!J90+Precision!J103+Precision!J116+Precision!J129)/10</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="44">
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>